<commit_message>
completed parent info extract
</commit_message>
<xml_diff>
--- a/record/maunal_records_base_case-dont-delete.xlsx
+++ b/record/maunal_records_base_case-dont-delete.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\chris\Documents\Personal\Personl Projects\Video-Processing\record\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F32A1E-09EF-4589-A517-2DC7011BA714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51700B75-2B1F-43C1-8CA1-DB20CF2594D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10665" yWindow="-14400" windowWidth="16410" windowHeight="14505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3225 (baseline)" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="580">
   <si>
     <t>Patient Name</t>
   </si>
@@ -1830,7 +1830,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1862,17 +1862,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1893,13 +1882,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1907,6 +1889,11 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2187,10 +2174,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F137"/>
+  <dimension ref="A1:G137"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2198,7 +2185,7 @@
     <col min="6" max="6" width="70.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2217,8 +2204,11 @@
       <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="12" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>142</v>
       </c>
@@ -2230,7 +2220,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>142</v>
       </c>
@@ -2242,7 +2232,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>142</v>
       </c>
@@ -2254,7 +2244,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>142</v>
       </c>
@@ -2266,7 +2256,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>142</v>
       </c>
@@ -2278,7 +2268,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>142</v>
       </c>
@@ -2290,7 +2280,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>142</v>
       </c>
@@ -2302,7 +2292,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>142</v>
       </c>
@@ -2314,7 +2304,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>143</v>
       </c>
@@ -2322,7 +2312,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>143</v>
       </c>
@@ -2330,7 +2320,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>143</v>
       </c>
@@ -2338,7 +2328,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>143</v>
       </c>
@@ -2346,7 +2336,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>143</v>
       </c>
@@ -2354,7 +2344,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -2362,7 +2352,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>143</v>
       </c>
@@ -3510,7 +3500,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>159</v>
       </c>
@@ -3518,7 +3508,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>159</v>
       </c>
@@ -3526,7 +3516,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>159</v>
       </c>
@@ -3534,7 +3524,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>159</v>
       </c>
@@ -3542,7 +3532,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>159</v>
       </c>
@@ -3550,7 +3540,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>159</v>
       </c>
@@ -3558,15 +3548,18 @@
         <v>138</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>159</v>
       </c>
       <c r="F135" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G135" s="11" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>159</v>
       </c>
@@ -3574,7 +3567,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>159</v>
       </c>
@@ -3590,10 +3583,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D4908A-C355-4E34-B1B6-03F1A2FC8F41}">
-  <dimension ref="A1:H145"/>
+  <dimension ref="A1:G145"/>
   <sheetViews>
-    <sheetView topLeftCell="B97" workbookViewId="0">
-      <selection activeCell="G133" sqref="G133"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3604,10 +3597,9 @@
     <col min="4" max="4" width="12" style="2" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="2"/>
     <col min="6" max="6" width="75.5703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>304</v>
       </c>
@@ -3626,44 +3618,26 @@
       <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="5" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F2" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="G2" s="8"/>
-    </row>
-    <row r="3" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F3" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="G3" s="8"/>
-    </row>
-    <row r="4" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F4" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="G4" s="8"/>
-    </row>
-    <row r="5" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2</v>
       </c>
@@ -3674,9 +3648,8 @@
       <c r="F5" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="G5" s="8"/>
-    </row>
-    <row r="6" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>2</v>
       </c>
@@ -3687,9 +3660,8 @@
       <c r="F6" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>2</v>
       </c>
@@ -3700,9 +3672,8 @@
       <c r="F7" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>2</v>
       </c>
@@ -3713,9 +3684,8 @@
       <c r="F8" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>2</v>
       </c>
@@ -3726,9 +3696,8 @@
       <c r="F9" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>2</v>
       </c>
@@ -3739,9 +3708,8 @@
       <c r="F10" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="G10" s="8"/>
-    </row>
-    <row r="11" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>2</v>
       </c>
@@ -3752,9 +3720,8 @@
       <c r="F11" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>2</v>
       </c>
@@ -3765,9 +3732,8 @@
       <c r="F12" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="G12" s="8"/>
-    </row>
-    <row r="13" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>2</v>
       </c>
@@ -3778,53 +3744,28 @@
       <c r="F13" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F14" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F15" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="G15" s="8"/>
-    </row>
-    <row r="16" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F16" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F17" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>4</v>
       </c>
@@ -3835,9 +3776,8 @@
       <c r="F18" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>4</v>
       </c>
@@ -3848,9 +3788,8 @@
       <c r="F19" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="G19" s="8"/>
-    </row>
-    <row r="20" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>4</v>
       </c>
@@ -3861,9 +3800,8 @@
       <c r="F20" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="G20" s="8"/>
-    </row>
-    <row r="21" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>4</v>
       </c>
@@ -3875,7 +3813,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="22" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>4</v>
       </c>
@@ -3887,7 +3825,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="23" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>4</v>
       </c>
@@ -3899,7 +3837,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="24" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>4</v>
       </c>
@@ -3911,7 +3849,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="25" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>4</v>
       </c>
@@ -3923,7 +3861,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="26" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>4</v>
       </c>
@@ -3935,7 +3873,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="27" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>4</v>
       </c>
@@ -3947,75 +3885,47 @@
         <v>185</v>
       </c>
     </row>
-    <row r="28" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F28" s="2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="29" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F29" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="30" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F30" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="31" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F31" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="32" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F32" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F33" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="H33"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F34" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="H34"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F35" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="H35"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>6</v>
       </c>
@@ -4026,9 +3936,8 @@
       <c r="F36" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="H36"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>6</v>
       </c>
@@ -4040,7 +3949,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>6</v>
       </c>
@@ -4052,7 +3961,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>6</v>
       </c>
@@ -4064,7 +3973,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>6</v>
       </c>
@@ -4076,7 +3985,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>6</v>
       </c>
@@ -4088,7 +3997,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>6</v>
       </c>
@@ -4100,7 +4009,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>6</v>
       </c>
@@ -4112,7 +4021,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>6</v>
       </c>
@@ -4124,7 +4033,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>6</v>
       </c>
@@ -4136,7 +4045,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>6</v>
       </c>
@@ -4148,7 +4057,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -4158,7 +4067,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F48" s="2" t="s">
         <v>206</v>
       </c>
@@ -4702,7 +4611,7 @@
       <c r="F114" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="G114" s="9" t="s">
+      <c r="G114" s="10" t="s">
         <v>307</v>
       </c>
     </row>
@@ -4710,7 +4619,7 @@
       <c r="F115" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="G115" s="9"/>
+      <c r="G115" s="10"/>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F116" s="2" t="s">
@@ -4741,7 +4650,7 @@
       <c r="F121" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="G121" s="10" t="s">
+      <c r="G121" s="7" t="s">
         <v>306</v>
       </c>
     </row>
@@ -4749,7 +4658,7 @@
       <c r="F122" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="G122" s="10" t="s">
+      <c r="G122" s="7" t="s">
         <v>306</v>
       </c>
     </row>
@@ -4757,7 +4666,7 @@
       <c r="F123" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="G123" s="10" t="s">
+      <c r="G123" s="7" t="s">
         <v>306</v>
       </c>
     </row>
@@ -4765,7 +4674,7 @@
       <c r="F124" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="G124" s="10" t="s">
+      <c r="G124" s="7" t="s">
         <v>306</v>
       </c>
     </row>
@@ -4803,7 +4712,7 @@
       <c r="F131" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="G131" s="10" t="s">
+      <c r="G131" s="7" t="s">
         <v>306</v>
       </c>
     </row>
@@ -4811,7 +4720,7 @@
       <c r="F132" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="G132" s="10" t="s">
+      <c r="G132" s="7" t="s">
         <v>306</v>
       </c>
     </row>
@@ -4819,7 +4728,7 @@
       <c r="F133" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="G133" s="10" t="s">
+      <c r="G133" s="7" t="s">
         <v>306</v>
       </c>
     </row>
@@ -4906,10 +4815,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>305</v>
       </c>
     </row>
@@ -5602,7 +5511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2284B17-57B1-4A51-8C10-7555E6877301}">
   <dimension ref="A1:B137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5610,10 +5519,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="9" t="s">
         <v>305</v>
       </c>
     </row>

</xml_diff>